<commit_message>
Version 5 figures and ms changes
</commit_message>
<xml_diff>
--- a/results/Supporting information/Table S3. Species x incubator traits summary.xlsx
+++ b/results/Supporting information/Table S3. Species x incubator traits summary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unioviedo-my.sharepoint.com/personal/espinosaclara_uniovi_es/Documents/IMIB/Softwares/GitHub/movealong/results/Supporting information/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="36" documentId="11_E7522FFD3007AB426011C11007C6599FF68AB09D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{53A2E681-D0C6-4ECF-BA60-454726DC7808}"/>
+  <xr:revisionPtr revIDLastSave="46" documentId="11_E7522FFD3007AB426011C11007C6599FF68AB09D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{82AD693F-4639-4E61-B3FC-F953A2371B64}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Temperate" sheetId="1" r:id="rId1"/>
@@ -875,7 +875,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -902,16 +902,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -926,12 +922,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -995,6 +996,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1297,10 +1302,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:R39"/>
+  <dimension ref="A1:R40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:D1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T36" sqref="T36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1311,54 +1316,56 @@
     <col min="5" max="11" width="6.85546875" customWidth="1"/>
     <col min="12" max="12" width="11.85546875" customWidth="1"/>
     <col min="13" max="14" width="6.85546875" customWidth="1"/>
-    <col min="15" max="15" width="17.5703125" customWidth="1"/>
-    <col min="16" max="16" width="16.85546875" customWidth="1"/>
+    <col min="15" max="15" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.7109375" customWidth="1"/>
+    <col min="17" max="17" width="13.42578125" customWidth="1"/>
+    <col min="18" max="18" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="12" t="s">
         <v>56</v>
       </c>
       <c r="B1" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="D1" s="20"/>
-      <c r="E1" s="11" t="s">
+      <c r="D1" s="19"/>
+      <c r="E1" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11" t="s">
+      <c r="F1" s="13"/>
+      <c r="G1" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11" t="s">
+      <c r="H1" s="13"/>
+      <c r="I1" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11" t="s">
+      <c r="J1" s="13"/>
+      <c r="K1" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11" t="s">
+      <c r="L1" s="13"/>
+      <c r="M1" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="N1" s="11"/>
-      <c r="O1" s="11" t="s">
+      <c r="N1" s="13"/>
+      <c r="O1" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="P1" s="11"/>
+      <c r="P1" s="13"/>
       <c r="Q1" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="R1" s="10" t="s">
+      <c r="R1" s="12" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="10"/>
+      <c r="A2" s="12"/>
       <c r="B2" s="17"/>
       <c r="C2" s="9" t="s">
         <v>64</v>
@@ -1403,17 +1410,17 @@
         <v>65</v>
       </c>
       <c r="Q2" s="15"/>
-      <c r="R2" s="10"/>
+      <c r="R2" s="12"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18" t="s">
+      <c r="C3" s="10"/>
+      <c r="D3" s="10" t="s">
         <v>89</v>
       </c>
       <c r="E3" s="2">
@@ -1463,13 +1470,13 @@
       <c r="A4" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="C4" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="D4" s="10" t="s">
         <v>90</v>
       </c>
       <c r="E4" s="2">
@@ -1519,13 +1526,13 @@
       <c r="A5" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="C5" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="D5" s="18" t="s">
+      <c r="D5" s="10" t="s">
         <v>90</v>
       </c>
       <c r="E5" s="2">
@@ -1575,13 +1582,13 @@
       <c r="A6" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="C6" s="18" t="s">
+      <c r="C6" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="D6" s="10" t="s">
         <v>89</v>
       </c>
       <c r="E6" s="2">
@@ -1621,7 +1628,7 @@
         <v>792</v>
       </c>
       <c r="Q6" s="2">
-        <f t="shared" ref="O6:Q39" si="0">N6-M6</f>
+        <f t="shared" ref="Q6:Q33" si="0">N6-M6</f>
         <v>22</v>
       </c>
       <c r="R6" s="5">
@@ -1632,13 +1639,13 @@
       <c r="A7" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="C7" s="18" t="s">
+      <c r="C7" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="D7" s="18" t="s">
+      <c r="D7" s="10" t="s">
         <v>89</v>
       </c>
       <c r="E7" s="2">
@@ -1689,13 +1696,13 @@
       <c r="A8" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="18" t="s">
+      <c r="B8" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="C8" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="D8" s="18" t="s">
+      <c r="D8" s="10" t="s">
         <v>89</v>
       </c>
       <c r="E8" s="2">
@@ -1746,13 +1753,13 @@
       <c r="A9" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="18" t="s">
+      <c r="B9" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="C9" s="18" t="s">
+      <c r="C9" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="D9" s="18" t="s">
+      <c r="D9" s="10" t="s">
         <v>92</v>
       </c>
       <c r="E9" s="2">
@@ -1803,13 +1810,13 @@
       <c r="A10" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="18" t="s">
+      <c r="B10" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="C10" s="18" t="s">
+      <c r="C10" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="D10" s="18" t="s">
+      <c r="D10" s="10" t="s">
         <v>91</v>
       </c>
       <c r="E10" s="2">
@@ -1860,13 +1867,13 @@
       <c r="A11" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="18" t="s">
+      <c r="B11" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="C11" s="18" t="s">
+      <c r="C11" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="D11" s="18" t="s">
+      <c r="D11" s="10" t="s">
         <v>92</v>
       </c>
       <c r="E11" s="2">
@@ -1916,13 +1923,13 @@
       <c r="A12" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B12" s="18" t="s">
+      <c r="B12" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="C12" s="18" t="s">
+      <c r="C12" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="D12" s="18" t="s">
+      <c r="D12" s="10" t="s">
         <v>90</v>
       </c>
       <c r="E12" s="2">
@@ -1973,13 +1980,13 @@
       <c r="A13" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B13" s="18" t="s">
+      <c r="B13" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="C13" s="18" t="s">
+      <c r="C13" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="D13" s="18"/>
+      <c r="D13" s="10"/>
       <c r="E13" s="2">
         <v>0</v>
       </c>
@@ -2016,13 +2023,13 @@
       <c r="A14" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B14" s="18" t="s">
+      <c r="B14" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="C14" s="18" t="s">
+      <c r="C14" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="D14" s="18" t="s">
+      <c r="D14" s="10" t="s">
         <v>92</v>
       </c>
       <c r="E14" s="2">
@@ -2119,13 +2126,13 @@
       <c r="A16" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="18" t="s">
+      <c r="B16" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="C16" s="18" t="s">
+      <c r="C16" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="D16" s="18" t="s">
+      <c r="D16" s="10" t="s">
         <v>89</v>
       </c>
       <c r="E16" s="2">
@@ -2176,13 +2183,13 @@
       <c r="A17" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B17" s="18" t="s">
+      <c r="B17" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="C17" s="18" t="s">
+      <c r="C17" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="D17" s="18" t="s">
+      <c r="D17" s="10" t="s">
         <v>90</v>
       </c>
       <c r="E17" s="2">
@@ -2232,13 +2239,13 @@
       <c r="A18" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B18" s="18" t="s">
+      <c r="B18" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="C18" s="18" t="s">
+      <c r="C18" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="D18" s="18" t="s">
+      <c r="D18" s="10" t="s">
         <v>90</v>
       </c>
       <c r="E18" s="2">
@@ -2289,13 +2296,13 @@
       <c r="A19" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B19" s="18" t="s">
+      <c r="B19" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="C19" s="18" t="s">
+      <c r="C19" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="D19" s="18" t="s">
+      <c r="D19" s="10" t="s">
         <v>92</v>
       </c>
       <c r="E19" s="2">
@@ -2346,13 +2353,13 @@
       <c r="A20" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B20" s="18" t="s">
+      <c r="B20" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="C20" s="18" t="s">
+      <c r="C20" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="D20" s="18" t="s">
+      <c r="D20" s="10" t="s">
         <v>89</v>
       </c>
       <c r="E20" s="2">
@@ -2403,13 +2410,13 @@
       <c r="A21" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B21" s="18" t="s">
+      <c r="B21" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="C21" s="18" t="s">
+      <c r="C21" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="D21" s="18" t="s">
+      <c r="D21" s="10" t="s">
         <v>89</v>
       </c>
       <c r="E21" s="2">
@@ -2460,13 +2467,13 @@
       <c r="A22" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B22" s="18" t="s">
+      <c r="B22" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="C22" s="18" t="s">
+      <c r="C22" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="D22" s="18" t="s">
+      <c r="D22" s="10" t="s">
         <v>92</v>
       </c>
       <c r="E22" s="2">
@@ -2564,13 +2571,13 @@
       <c r="A24" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B24" s="18" t="s">
+      <c r="B24" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="C24" s="18" t="s">
+      <c r="C24" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="D24" s="18" t="s">
+      <c r="D24" s="10" t="s">
         <v>90</v>
       </c>
       <c r="E24" s="2">
@@ -2621,13 +2628,13 @@
       <c r="A25" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B25" s="18" t="s">
+      <c r="B25" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="C25" s="18" t="s">
+      <c r="C25" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="D25" s="18" t="s">
+      <c r="D25" s="10" t="s">
         <v>89</v>
       </c>
       <c r="E25" s="2">
@@ -2677,13 +2684,13 @@
       <c r="A26" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B26" s="18" t="s">
+      <c r="B26" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="C26" s="18" t="s">
+      <c r="C26" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="D26" s="18" t="s">
+      <c r="D26" s="10" t="s">
         <v>90</v>
       </c>
       <c r="E26" s="2">
@@ -2733,13 +2740,13 @@
       <c r="A27" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B27" s="18" t="s">
+      <c r="B27" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="C27" s="18" t="s">
+      <c r="C27" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="D27" s="18" t="s">
+      <c r="D27" s="10" t="s">
         <v>92</v>
       </c>
       <c r="E27" s="2">
@@ -2790,13 +2797,13 @@
       <c r="A28" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B28" s="18" t="s">
+      <c r="B28" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="C28" s="18" t="s">
+      <c r="C28" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="D28" s="18" t="s">
+      <c r="D28" s="10" t="s">
         <v>92</v>
       </c>
       <c r="E28" s="2">
@@ -2846,13 +2853,13 @@
       <c r="A29" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B29" s="18" t="s">
+      <c r="B29" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="C29" s="18" t="s">
+      <c r="C29" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="D29" s="18" t="s">
+      <c r="D29" s="10" t="s">
         <v>92</v>
       </c>
       <c r="E29" s="2">
@@ -2903,13 +2910,13 @@
       <c r="A30" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B30" s="18" t="s">
+      <c r="B30" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="C30" s="18" t="s">
+      <c r="C30" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="D30" s="18"/>
+      <c r="D30" s="10"/>
       <c r="E30" s="2">
         <v>0</v>
       </c>
@@ -3002,13 +3009,13 @@
       <c r="A32" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B32" s="18" t="s">
+      <c r="B32" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="C32" s="18" t="s">
+      <c r="C32" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="D32" s="18" t="s">
+      <c r="D32" s="10" t="s">
         <v>89</v>
       </c>
       <c r="E32" s="2">
@@ -3059,13 +3066,13 @@
       <c r="A33" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B33" s="18" t="s">
+      <c r="B33" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="C33" s="18" t="s">
+      <c r="C33" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="D33" s="18" t="s">
+      <c r="D33" s="10" t="s">
         <v>89</v>
       </c>
       <c r="E33" s="2">
@@ -3116,13 +3123,13 @@
       <c r="A34" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B34" s="18" t="s">
+      <c r="B34" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="C34" s="18" t="s">
+      <c r="C34" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="D34" s="18" t="s">
+      <c r="D34" s="10" t="s">
         <v>89</v>
       </c>
       <c r="E34" s="2">
@@ -3219,11 +3226,11 @@
       <c r="A36" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B36" s="18" t="s">
+      <c r="B36" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="C36" s="18"/>
-      <c r="D36" s="18"/>
+      <c r="C36" s="10"/>
+      <c r="D36" s="10"/>
       <c r="E36" s="2">
         <v>93.33</v>
       </c>
@@ -3272,11 +3279,11 @@
       <c r="A37" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B37" s="18" t="s">
+      <c r="B37" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="C37" s="18"/>
-      <c r="D37" s="18"/>
+      <c r="C37" s="10"/>
+      <c r="D37" s="10"/>
       <c r="E37" s="2">
         <v>6.0650000000000004</v>
       </c>
@@ -3325,11 +3332,11 @@
       <c r="A38" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B38" s="18" t="s">
+      <c r="B38" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="C38" s="18"/>
-      <c r="D38" s="18"/>
+      <c r="C38" s="10"/>
+      <c r="D38" s="10"/>
       <c r="E38" s="2">
         <v>10</v>
       </c>
@@ -3378,11 +3385,11 @@
       <c r="A39" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B39" s="18" t="s">
+      <c r="B39" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="C39" s="18"/>
-      <c r="D39" s="18"/>
+      <c r="C39" s="10"/>
+      <c r="D39" s="10"/>
       <c r="E39" s="2">
         <v>52.255000000000003</v>
       </c>
@@ -3426,6 +3433,9 @@
       <c r="R39" s="5">
         <v>151.82660000000001</v>
       </c>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="Q40" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -3448,10 +3458,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:R23"/>
+  <dimension ref="A1:R24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:D1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q24" sqref="Q24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3465,49 +3475,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="12" t="s">
         <v>56</v>
       </c>
       <c r="B1" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="D1" s="20"/>
-      <c r="E1" s="11" t="s">
+      <c r="D1" s="19"/>
+      <c r="E1" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11" t="s">
+      <c r="F1" s="13"/>
+      <c r="G1" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11" t="s">
+      <c r="H1" s="13"/>
+      <c r="I1" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11" t="s">
+      <c r="J1" s="13"/>
+      <c r="K1" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11" t="s">
+      <c r="L1" s="13"/>
+      <c r="M1" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="N1" s="11"/>
-      <c r="O1" s="11" t="s">
+      <c r="N1" s="13"/>
+      <c r="O1" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="P1" s="11"/>
-      <c r="Q1" s="12" t="s">
+      <c r="P1" s="13"/>
+      <c r="Q1" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="R1" s="10" t="s">
+      <c r="R1" s="12" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:18" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="10"/>
+      <c r="A2" s="12"/>
       <c r="B2" s="17"/>
       <c r="C2" s="9" t="s">
         <v>64</v>
@@ -3551,20 +3561,20 @@
       <c r="P2" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="Q2" s="13"/>
-      <c r="R2" s="10"/>
+      <c r="Q2" s="21"/>
+      <c r="R2" s="12"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="D3" s="10" t="s">
         <v>91</v>
       </c>
       <c r="E3" s="2">
@@ -3615,13 +3625,13 @@
       <c r="A4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="C4" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="D4" s="10" t="s">
         <v>90</v>
       </c>
       <c r="E4" s="2">
@@ -3672,13 +3682,13 @@
       <c r="A5" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="C5" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="D5" s="18" t="s">
+      <c r="D5" s="10" t="s">
         <v>90</v>
       </c>
       <c r="E5" s="2">
@@ -3729,13 +3739,13 @@
       <c r="A6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="C6" s="18" t="s">
+      <c r="C6" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="D6" s="10" t="s">
         <v>92</v>
       </c>
       <c r="E6" s="2">
@@ -3786,13 +3796,13 @@
       <c r="A7" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="C7" s="18" t="s">
+      <c r="C7" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="D7" s="18" t="s">
+      <c r="D7" s="10" t="s">
         <v>90</v>
       </c>
       <c r="E7" s="2">
@@ -3843,13 +3853,13 @@
       <c r="A8" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="18" t="s">
+      <c r="B8" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="C8" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="D8" s="18" t="s">
+      <c r="D8" s="10" t="s">
         <v>90</v>
       </c>
       <c r="E8" s="2">
@@ -3900,13 +3910,13 @@
       <c r="A9" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="18" t="s">
+      <c r="B9" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="C9" s="18" t="s">
+      <c r="C9" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="D9" s="18" t="s">
+      <c r="D9" s="10" t="s">
         <v>89</v>
       </c>
       <c r="E9" s="2">
@@ -3957,13 +3967,13 @@
       <c r="A10" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="18" t="s">
+      <c r="B10" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="C10" s="18" t="s">
+      <c r="C10" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="D10" s="18" t="s">
+      <c r="D10" s="10" t="s">
         <v>92</v>
       </c>
       <c r="E10" s="2">
@@ -4014,13 +4024,13 @@
       <c r="A11" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="18" t="s">
+      <c r="B11" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="C11" s="18" t="s">
+      <c r="C11" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="D11" s="18" t="s">
+      <c r="D11" s="10" t="s">
         <v>92</v>
       </c>
       <c r="E11" s="2">
@@ -4071,13 +4081,13 @@
       <c r="A12" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="18" t="s">
+      <c r="B12" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="C12" s="18" t="s">
+      <c r="C12" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="D12" s="18" t="s">
+      <c r="D12" s="10" t="s">
         <v>90</v>
       </c>
       <c r="E12" s="2">
@@ -4128,13 +4138,13 @@
       <c r="A13" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="18" t="s">
+      <c r="B13" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="C13" s="18" t="s">
+      <c r="C13" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="D13" s="18" t="s">
+      <c r="D13" s="10" t="s">
         <v>90</v>
       </c>
       <c r="E13" s="2">
@@ -4185,13 +4195,13 @@
       <c r="A14" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="18" t="s">
+      <c r="B14" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="C14" s="18" t="s">
+      <c r="C14" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="D14" s="18" t="s">
+      <c r="D14" s="10" t="s">
         <v>90</v>
       </c>
       <c r="E14" s="2">
@@ -4242,13 +4252,13 @@
       <c r="A15" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="18" t="s">
+      <c r="B15" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="C15" s="18" t="s">
+      <c r="C15" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="D15" s="18" t="s">
+      <c r="D15" s="10" t="s">
         <v>91</v>
       </c>
       <c r="E15" s="2">
@@ -4298,13 +4308,13 @@
       <c r="A16" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="18" t="s">
+      <c r="B16" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="C16" s="18" t="s">
+      <c r="C16" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="D16" s="18" t="s">
+      <c r="D16" s="10" t="s">
         <v>90</v>
       </c>
       <c r="E16" s="2">
@@ -4355,13 +4365,13 @@
       <c r="A17" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="18" t="s">
+      <c r="B17" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="C17" s="18" t="s">
+      <c r="C17" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="D17" s="18" t="s">
+      <c r="D17" s="10" t="s">
         <v>90</v>
       </c>
       <c r="E17" s="2">
@@ -4412,13 +4422,13 @@
       <c r="A18" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="18" t="s">
+      <c r="B18" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="C18" s="18" t="s">
+      <c r="C18" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="D18" s="18" t="s">
+      <c r="D18" s="10" t="s">
         <v>90</v>
       </c>
       <c r="E18" s="2">
@@ -4469,13 +4479,13 @@
       <c r="A19" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="18" t="s">
+      <c r="B19" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="C19" s="18" t="s">
+      <c r="C19" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="D19" s="18" t="s">
+      <c r="D19" s="10" t="s">
         <v>89</v>
       </c>
       <c r="E19" s="2">
@@ -4526,13 +4536,13 @@
       <c r="A20" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="18" t="s">
+      <c r="B20" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="C20" s="18" t="s">
+      <c r="C20" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="D20" s="18" t="s">
+      <c r="D20" s="10" t="s">
         <v>91</v>
       </c>
       <c r="E20" s="2">
@@ -4583,13 +4593,13 @@
       <c r="A21" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="18" t="s">
+      <c r="B21" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="C21" s="18" t="s">
+      <c r="C21" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="D21" s="18" t="s">
+      <c r="D21" s="10" t="s">
         <v>92</v>
       </c>
       <c r="E21" s="2">
@@ -4640,13 +4650,13 @@
       <c r="A22" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="18" t="s">
+      <c r="B22" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="C22" s="18" t="s">
+      <c r="C22" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="D22" s="18" t="s">
+      <c r="D22" s="10" t="s">
         <v>90</v>
       </c>
       <c r="E22" s="2">
@@ -4697,13 +4707,13 @@
       <c r="A23" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="18" t="s">
+      <c r="B23" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="C23" s="18" t="s">
+      <c r="C23" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="D23" s="18" t="s">
+      <c r="D23" s="10" t="s">
         <v>90</v>
       </c>
       <c r="E23" s="2">
@@ -4749,6 +4759,9 @@
       <c r="R23" s="5">
         <v>65.792850000000001</v>
       </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="Q24" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="11">

</xml_diff>

<commit_message>
last version with updated conclusion
</commit_message>
<xml_diff>
--- a/results/Supporting information/Table S3. Species x incubator traits summary.xlsx
+++ b/results/Supporting information/Table S3. Species x incubator traits summary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unioviedo-my.sharepoint.com/personal/espinosaclara_uniovi_es/Documents/IMIB/Softwares/GitHub/movealong/results/Supporting information/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="46" documentId="11_E7522FFD3007AB426011C11007C6599FF68AB09D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{82AD693F-4639-4E61-B3FC-F953A2371B64}"/>
+  <xr:revisionPtr revIDLastSave="50" documentId="11_E7522FFD3007AB426011C11007C6599FF68AB09D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3DAC4643-83F8-4785-9199-660963D5B0FC}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Temperate" sheetId="1" r:id="rId1"/>
@@ -1304,8 +1304,8 @@
   </sheetPr>
   <dimension ref="A1:R40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T36" sqref="T36"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="Q40" sqref="Q40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3460,8 +3460,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:R24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q24" sqref="Q24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q27" sqref="Q27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Ecology Letters submission formating
</commit_message>
<xml_diff>
--- a/results/Supporting information/Table S3. Species x incubator traits summary.xlsx
+++ b/results/Supporting information/Table S3. Species x incubator traits summary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unioviedo-my.sharepoint.com/personal/espinosaclara_uniovi_es/Documents/IMIB/Softwares/GitHub/movealong/results/Supporting information/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unioviedo-my.sharepoint.com/personal/espinosaclara_uniovi_es/Documents/IMIB/Softwares/GitHub/Germination_phenology/results/Supporting information/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="50" documentId="11_E7522FFD3007AB426011C11007C6599FF68AB09D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3DAC4643-83F8-4785-9199-660963D5B0FC}"/>
+  <xr:revisionPtr revIDLastSave="54" documentId="11_E7522FFD3007AB426011C11007C6599FF68AB09D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C293C168-9D77-41FC-A66F-B4A0C63887EE}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Temperate" sheetId="1" r:id="rId1"/>
@@ -1302,10 +1302,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:R40"/>
+  <dimension ref="A1:S40"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="Q40" sqref="Q40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S16" sqref="S16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1322,7 +1322,7 @@
     <col min="18" max="18" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>56</v>
       </c>
@@ -1364,7 +1364,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12"/>
       <c r="B2" s="17"/>
       <c r="C2" s="9" t="s">
@@ -1412,7 +1412,7 @@
       <c r="Q2" s="15"/>
       <c r="R2" s="12"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>22</v>
       </c>
@@ -1465,8 +1465,12 @@
       <c r="R3" s="5">
         <v>-0.63234170000000001</v>
       </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S3" s="11" t="e">
+        <f>AVERAGE(M3:N3)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>23</v>
       </c>
@@ -1521,8 +1525,12 @@
       <c r="R4" s="5">
         <v>12.15582</v>
       </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S4" s="11" t="e">
+        <f t="shared" ref="S4:S39" si="0">AVERAGE(M4:N4)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>24</v>
       </c>
@@ -1577,8 +1585,12 @@
       <c r="R5" s="5">
         <v>69.102739999999997</v>
       </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S5" s="11" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>25</v>
       </c>
@@ -1628,14 +1640,18 @@
         <v>792</v>
       </c>
       <c r="Q6" s="2">
-        <f t="shared" ref="Q6:Q33" si="0">N6-M6</f>
+        <f t="shared" ref="Q6:Q33" si="1">N6-M6</f>
         <v>22</v>
       </c>
       <c r="R6" s="5">
         <v>30.777899999999999</v>
       </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S6" s="11">
+        <f t="shared" si="0"/>
+        <v>283</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>26</v>
       </c>
@@ -1685,14 +1701,18 @@
         <v>596.75</v>
       </c>
       <c r="Q7" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>39.801388888888994</v>
       </c>
       <c r="R7" s="5">
         <v>30.845549999999999</v>
       </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S7" s="11">
+        <f t="shared" si="0"/>
+        <v>258.10277777777753</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>27</v>
       </c>
@@ -1742,14 +1762,18 @@
         <v>548.3125</v>
       </c>
       <c r="Q8" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>38.043102073364992</v>
       </c>
       <c r="R8" s="5">
         <v>38.153109999999998</v>
       </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S8" s="11">
+        <f t="shared" si="0"/>
+        <v>263.87780103668251</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>28</v>
       </c>
@@ -1799,14 +1823,18 @@
         <v>251.875</v>
       </c>
       <c r="Q9" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>17.501092657343008</v>
       </c>
       <c r="R9" s="5">
         <v>11.870900000000001</v>
       </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S9" s="11">
+        <f t="shared" si="0"/>
+        <v>221.68179632867151</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>29</v>
       </c>
@@ -1856,14 +1884,18 @@
         <v>325.125</v>
       </c>
       <c r="Q10" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>41.892647058824025</v>
       </c>
       <c r="R10" s="5">
         <v>43.796329999999998</v>
       </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S10" s="11">
+        <f t="shared" si="0"/>
+        <v>240.69632352941201</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>30</v>
       </c>
@@ -1918,8 +1950,12 @@
       <c r="R11" s="5">
         <v>7.7578389999999997E-2</v>
       </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S11" s="11" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>31</v>
       </c>
@@ -1969,14 +2005,18 @@
         <v>178</v>
       </c>
       <c r="Q12" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>107.739583333333</v>
       </c>
       <c r="R12" s="5">
         <v>83.157409999999999</v>
       </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S12" s="11">
+        <f t="shared" si="0"/>
+        <v>68.963541666666501</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>32</v>
       </c>
@@ -2012,14 +2052,18 @@
       </c>
       <c r="P13" s="2"/>
       <c r="Q13" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-239.5</v>
       </c>
       <c r="R13" s="7" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S13" s="11">
+        <f t="shared" si="0"/>
+        <v>239.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>33</v>
       </c>
@@ -2074,8 +2118,12 @@
       <c r="R14" s="5">
         <v>1.2084980000000001</v>
       </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S14" s="11" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>34</v>
       </c>
@@ -2121,8 +2169,12 @@
       <c r="R15" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S15" s="11" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>35</v>
       </c>
@@ -2172,14 +2224,18 @@
         <v>523.125</v>
       </c>
       <c r="Q16" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>51.553265668154978</v>
       </c>
       <c r="R16" s="5">
         <v>75.370099999999994</v>
       </c>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S16" s="11">
+        <f t="shared" si="0"/>
+        <v>256.0370495007445</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>36</v>
       </c>
@@ -2234,8 +2290,12 @@
       <c r="R17" s="5">
         <v>29.819759999999999</v>
       </c>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S17" s="11">
+        <f t="shared" si="0"/>
+        <v>279</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>37</v>
       </c>
@@ -2285,14 +2345,18 @@
         <v>91</v>
       </c>
       <c r="Q18" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.4401041666666003</v>
       </c>
       <c r="R18" s="5">
         <v>-32.509419999999999</v>
       </c>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S18" s="11">
+        <f t="shared" si="0"/>
+        <v>14.03515625</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>38</v>
       </c>
@@ -2342,14 +2406,18 @@
         <v>277</v>
       </c>
       <c r="Q19" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.0187500000000114</v>
       </c>
       <c r="R19" s="5">
         <v>23.03575</v>
       </c>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S19" s="11">
+        <f t="shared" si="0"/>
+        <v>230.57187500000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>39</v>
       </c>
@@ -2399,14 +2467,18 @@
         <v>1005.875</v>
       </c>
       <c r="Q20" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>302.11065423976595</v>
       </c>
       <c r="R20" s="5">
         <v>183.4111</v>
       </c>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S20" s="11">
+        <f t="shared" si="0"/>
+        <v>160.618283991228</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>40</v>
       </c>
@@ -2456,14 +2528,18 @@
         <v>474.25</v>
       </c>
       <c r="Q21" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>46.041666666667027</v>
       </c>
       <c r="R21" s="5">
         <v>14.02195</v>
       </c>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S21" s="11">
+        <f t="shared" si="0"/>
+        <v>249.27083333333351</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>7</v>
       </c>
@@ -2513,14 +2589,18 @@
         <v>268.5</v>
       </c>
       <c r="Q22" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>110.916666666667</v>
       </c>
       <c r="R22" s="5">
         <v>94.146439999999998</v>
       </c>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S22" s="11">
+        <f t="shared" si="0"/>
+        <v>175.04166666666652</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
         <v>41</v>
       </c>
@@ -2566,8 +2646,12 @@
       <c r="R23" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S23" s="11" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>42</v>
       </c>
@@ -2617,14 +2701,18 @@
         <v>185.9375</v>
       </c>
       <c r="Q24" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>17.894845085470099</v>
       </c>
       <c r="R24" s="5">
         <v>54.54562</v>
       </c>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S24" s="11">
+        <f t="shared" si="0"/>
+        <v>21.080755876068352</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>43</v>
       </c>
@@ -2679,8 +2767,12 @@
       <c r="R25" s="5">
         <v>97.170490000000001</v>
       </c>
-    </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S25" s="11">
+        <f t="shared" si="0"/>
+        <v>227</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>44</v>
       </c>
@@ -2735,8 +2827,12 @@
       <c r="R26" s="5">
         <v>112.3931</v>
       </c>
-    </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S26" s="11" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>45</v>
       </c>
@@ -2786,14 +2882,18 @@
         <v>334</v>
       </c>
       <c r="Q27" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>45.78333333333299</v>
       </c>
       <c r="R27" s="5">
         <v>21.053730000000002</v>
       </c>
-    </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S27" s="11">
+        <f t="shared" si="0"/>
+        <v>226.55833333333351</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>46</v>
       </c>
@@ -2848,8 +2948,12 @@
       <c r="R28" s="5">
         <v>-11.422639999999999</v>
       </c>
-    </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S28" s="11" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>47</v>
       </c>
@@ -2899,14 +3003,18 @@
         <v>225.333333333333</v>
       </c>
       <c r="Q29" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>58.515758547008005</v>
       </c>
       <c r="R29" s="5">
         <v>82.974209999999999</v>
       </c>
-    </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S29" s="11">
+        <f t="shared" si="0"/>
+        <v>205.28795405982902</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>48</v>
       </c>
@@ -2959,8 +3067,12 @@
       <c r="R30" s="5">
         <v>24.668749999999999</v>
       </c>
-    </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S30" s="11" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
         <v>49</v>
       </c>
@@ -3004,8 +3116,12 @@
       <c r="R31" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S31" s="11" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>50</v>
       </c>
@@ -3055,14 +3171,18 @@
         <v>1284.6666666666699</v>
       </c>
       <c r="Q32" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>265.06246565934072</v>
       </c>
       <c r="R32" s="5">
         <v>195.16929999999999</v>
       </c>
-    </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S32" s="11">
+        <f t="shared" si="0"/>
+        <v>195.06876717032966</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>51</v>
       </c>
@@ -3112,14 +3232,18 @@
         <v>551.5</v>
       </c>
       <c r="Q33" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>61.502252700321975</v>
       </c>
       <c r="R33" s="5">
         <v>84.829350000000005</v>
       </c>
-    </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S33" s="11">
+        <f t="shared" si="0"/>
+        <v>252.76871491968001</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>52</v>
       </c>
@@ -3174,8 +3298,12 @@
       <c r="R34" s="5">
         <v>-1.361059</v>
       </c>
-    </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S34" s="11" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="s">
         <v>53</v>
       </c>
@@ -3221,8 +3349,12 @@
       <c r="R35" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S35" s="11" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>54</v>
       </c>
@@ -3274,8 +3406,12 @@
       <c r="R36" s="5">
         <v>146.8434</v>
       </c>
-    </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S36" s="11">
+        <f t="shared" si="0"/>
+        <v>110.2564503205128</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>55</v>
       </c>
@@ -3327,8 +3463,12 @@
       <c r="R37" s="5">
         <v>17.534929999999999</v>
       </c>
-    </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S37" s="11">
+        <f t="shared" si="0"/>
+        <v>295.95833333333348</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>18</v>
       </c>
@@ -3380,8 +3520,12 @@
       <c r="R38" s="5">
         <v>56.58296</v>
       </c>
-    </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S38" s="11">
+        <f t="shared" si="0"/>
+        <v>233.33159722222251</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>21</v>
       </c>
@@ -3433,8 +3577,12 @@
       <c r="R39" s="5">
         <v>151.82660000000001</v>
       </c>
-    </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S39" s="11">
+        <f t="shared" si="0"/>
+        <v>198.354052986326</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
       <c r="Q40" s="11"/>
     </row>
   </sheetData>
@@ -3458,10 +3606,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:R24"/>
+  <dimension ref="A1:S24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q27" sqref="Q27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="S23" sqref="S23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3474,7 +3622,7 @@
     <col min="15" max="15" width="9.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>56</v>
       </c>
@@ -3516,7 +3664,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:18" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12"/>
       <c r="B2" s="17"/>
       <c r="C2" s="9" t="s">
@@ -3564,7 +3712,7 @@
       <c r="Q2" s="21"/>
       <c r="R2" s="12"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
@@ -3620,8 +3768,12 @@
       <c r="R3" s="5">
         <v>69.814580000000007</v>
       </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S3" s="11">
+        <f>AVERAGE(M3:N3)</f>
+        <v>263.5625</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>1</v>
       </c>
@@ -3677,8 +3829,12 @@
       <c r="R4" s="5">
         <v>25.44096</v>
       </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S4" s="11">
+        <f t="shared" ref="S4:S23" si="1">AVERAGE(M4:N4)</f>
+        <v>11.2507316136857</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>2</v>
       </c>
@@ -3734,8 +3890,12 @@
       <c r="R5" s="5">
         <v>-8.0269919999999999</v>
       </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S5" s="11">
+        <f t="shared" si="1"/>
+        <v>48.436965505899352</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>3</v>
       </c>
@@ -3791,8 +3951,12 @@
       <c r="R6" s="5">
         <v>29.18449</v>
       </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S6" s="11">
+        <f t="shared" si="1"/>
+        <v>223.30639880952401</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>4</v>
       </c>
@@ -3848,8 +4012,12 @@
       <c r="R7" s="5">
         <v>6.1222849999999998</v>
       </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S7" s="11">
+        <f t="shared" si="1"/>
+        <v>4.5486126150975297</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>5</v>
       </c>
@@ -3905,8 +4073,12 @@
       <c r="R8" s="5">
         <v>17.046119999999998</v>
       </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S8" s="11">
+        <f t="shared" si="1"/>
+        <v>20.768308692941048</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>6</v>
       </c>
@@ -3962,8 +4134,12 @@
       <c r="R9" s="5">
         <v>34.588180000000001</v>
       </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S9" s="11">
+        <f t="shared" si="1"/>
+        <v>154.21354166666652</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>7</v>
       </c>
@@ -4019,8 +4195,12 @@
       <c r="R10" s="5">
         <v>191.21639999999999</v>
       </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S10" s="11">
+        <f t="shared" si="1"/>
+        <v>128.10520833333334</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>8</v>
       </c>
@@ -4076,8 +4256,12 @@
       <c r="R11" s="5">
         <v>107.0115</v>
       </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S11" s="11">
+        <f t="shared" si="1"/>
+        <v>173.95039682539701</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>9</v>
       </c>
@@ -4133,8 +4317,12 @@
       <c r="R12" s="5">
         <v>54.196770000000001</v>
       </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S12" s="11">
+        <f t="shared" si="1"/>
+        <v>10.03510456100917</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>10</v>
       </c>
@@ -4190,8 +4378,12 @@
       <c r="R13" s="5">
         <v>17.603860000000001</v>
       </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S13" s="11">
+        <f t="shared" si="1"/>
+        <v>7.7991652632713002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>11</v>
       </c>
@@ -4247,8 +4439,12 @@
       <c r="R14" s="5">
         <v>2.7350300000000001</v>
       </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S14" s="11">
+        <f t="shared" si="1"/>
+        <v>61.190251426091251</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>12</v>
       </c>
@@ -4303,8 +4499,12 @@
       <c r="R15" s="5">
         <v>10.14752</v>
       </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S15" s="11">
+        <f t="shared" si="1"/>
+        <v>284.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>14</v>
       </c>
@@ -4360,8 +4560,12 @@
       <c r="R16" s="5">
         <v>8.8713510000000007</v>
       </c>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S16" s="11">
+        <f t="shared" si="1"/>
+        <v>8.2387290019762851</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>15</v>
       </c>
@@ -4417,8 +4621,12 @@
       <c r="R17" s="5">
         <v>62.859369999999998</v>
       </c>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S17" s="11">
+        <f t="shared" si="1"/>
+        <v>124.94626736111115</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>16</v>
       </c>
@@ -4474,8 +4682,12 @@
       <c r="R18" s="5">
         <v>28.353670000000001</v>
       </c>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S18" s="11">
+        <f t="shared" si="1"/>
+        <v>79.970467032967008</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>17</v>
       </c>
@@ -4531,8 +4743,12 @@
       <c r="R19" s="5">
         <v>55.334409999999998</v>
       </c>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S19" s="11">
+        <f t="shared" si="1"/>
+        <v>236.27040112665151</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>18</v>
       </c>
@@ -4588,8 +4804,12 @@
       <c r="R20" s="5">
         <v>30.549150000000001</v>
       </c>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S20" s="11">
+        <f t="shared" si="1"/>
+        <v>219.82366217320251</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>19</v>
       </c>
@@ -4645,8 +4865,12 @@
       <c r="R21" s="5">
         <v>164.5787</v>
       </c>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S21" s="11">
+        <f t="shared" si="1"/>
+        <v>125.08853744294896</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>20</v>
       </c>
@@ -4702,8 +4926,12 @@
       <c r="R22" s="5">
         <v>-62.093020000000003</v>
       </c>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S22" s="11">
+        <f t="shared" si="1"/>
+        <v>101.9896786236424</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>21</v>
       </c>
@@ -4759,8 +4987,12 @@
       <c r="R23" s="5">
         <v>65.792850000000001</v>
       </c>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S23" s="11">
+        <f t="shared" si="1"/>
+        <v>48.598741908622401</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="Q24" s="11"/>
     </row>
   </sheetData>

</xml_diff>